<commit_message>
Added Spreadsheets and episode Links
</commit_message>
<xml_diff>
--- a/notebooks/SOSNEP03LR.xlsx
+++ b/notebooks/SOSNEP03LR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwoody\repos\dataexposed\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266E2F78-0CD5-43FD-BA3D-149AC72711F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9B0066-743E-4FD6-82B3-DE06EBA9FF19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60960" yWindow="1365" windowWidth="33885" windowHeight="20235" tabRatio="255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" tabRatio="255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Salary</t>
   </si>
@@ -135,12 +135,48 @@
   <si>
     <t>Salary Analysis</t>
   </si>
+  <si>
+    <t>xy</t>
+  </si>
+  <si>
+    <t>x^2</t>
+  </si>
+  <si>
+    <t>y^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 2: Find the M and B: </t>
+  </si>
+  <si>
+    <t>Step 1: Set up the x's and y's and their multiples/sums:</t>
+  </si>
+  <si>
+    <t>Sums</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = </t>
+  </si>
+  <si>
+    <t>Step 3: Build the Formula y=a+bx:</t>
+  </si>
+  <si>
+    <t>y=3.63E-10*1.46E-11*x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +315,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -465,7 +509,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -600,6 +644,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -645,7 +698,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -655,6 +708,18 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="13" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -700,7 +765,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1873,26 +1945,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
@@ -2005,26 +2057,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
@@ -2164,597 +2196,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2"/>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2796,6 +2237,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>165925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>30544</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18751A14-8596-4E1B-AA4E-449D594F249B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6339840" y="929640"/>
+          <a:ext cx="1362265" cy="457264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381223</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>211517</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BEE25EA-BF1E-4A66-9AAE-80DD79EE3054}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6316980" y="190500"/>
+          <a:ext cx="1600423" cy="447737"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{4798D577-8BA0-4855-8170-55CE9DB8CD2C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="3">
@@ -2819,11 +2353,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96C00DCA-223E-4D8B-874A-3C82134268FB}" name="Table1" displayName="Table1" ref="A1:B75" totalsRowShown="0">
-  <autoFilter ref="A1:B75" xr:uid="{E653397B-9E31-445D-BCF9-D70171F5FF81}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96C00DCA-223E-4D8B-874A-3C82134268FB}" name="Table1" displayName="Table1" ref="A2:B77" totalsRowCount="1">
+  <autoFilter ref="A2:B76" xr:uid="{E653397B-9E31-445D-BCF9-D70171F5FF81}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BD229110-C4B0-4A5A-9015-D3C0B6CCFC46}" name="Salary"/>
-    <tableColumn id="2" xr3:uid="{E9C972DA-372D-4565-AC84-2243F0624B27}" name="Years Employed"/>
+    <tableColumn id="1" xr3:uid="{BD229110-C4B0-4A5A-9015-D3C0B6CCFC46}" name="Salary" totalsRowFunction="custom" totalsRowDxfId="1">
+      <totalsRowFormula>SUM(A3:A76)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{E9C972DA-372D-4565-AC84-2243F0624B27}" name="Years Employed" totalsRowFunction="custom" totalsRowDxfId="0">
+      <totalsRowFormula>SUM(B3:B76)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3129,7 +2667,7 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4185,7 +3723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31298BB-59EF-4CC6-8F3B-369433AA5061}">
   <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -4805,622 +4343,1637 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.88671875" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="P1" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="D2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="10">
+        <f>(Table1[[#Totals],[Salary]]*E77)-(Table1[[#Totals],[Years Employed]]*D77)</f>
+        <v>652027398.57492065</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="9">
+        <f>L2/L3</f>
+        <v>3.63011599035688E-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>119980</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="D3" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1439760</v>
+      </c>
+      <c r="E3" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>144</v>
+      </c>
+      <c r="F3" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>14395200400</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9">
+        <f>(COUNT(Table1[Salary])*(D77^2))-((Table1[[#Totals],[Years Employed]]^2))</f>
+        <v>1.7961613356349509E+18</v>
+      </c>
+      <c r="M3" s="9"/>
+      <c r="P3" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>116480</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>12.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="D4" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1467648</v>
+      </c>
+      <c r="E4" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>158.76</v>
+      </c>
+      <c r="F4" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>13567590400</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>123200</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>12.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="D5" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1564640</v>
+      </c>
+      <c r="E5" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>161.29</v>
+      </c>
+      <c r="F5" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15178240000</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9">
+        <f>(COUNT(Table1[Salary])*(D77))-(Table1[[#Totals],[Years Employed]]*Table1[[#Totals],[Salary]])</f>
+        <v>26328511.999998093</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="9">
+        <f>L5/L6</f>
+        <v>1.4658211084746934E-11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>117950</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>13.700000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="D6" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1615915.0000000002</v>
+      </c>
+      <c r="E6" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>187.69000000000003</v>
+      </c>
+      <c r="F6" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>13912202500</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9">
+        <f>(COUNT(Table1[Salary])*(D77^2))-(Table1[[#Totals],[Years Employed]]^2)</f>
+        <v>1.7961613356349509E+18</v>
+      </c>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>118510</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>14.15</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="D7" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1676916.5</v>
+      </c>
+      <c r="E7" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>200.2225</v>
+      </c>
+      <c r="F7" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>14044620100</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>116900</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>14.55</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>123480</v>
-      </c>
-      <c r="B8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D8" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1700895</v>
+      </c>
+      <c r="E8" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>211.70250000000001</v>
+      </c>
+      <c r="F8" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>13665610000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>123480</v>
       </c>
       <c r="B9">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D9" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1852200</v>
+      </c>
+      <c r="E9" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>225</v>
+      </c>
+      <c r="F9" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15247310400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
+        <v>123480</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="D10" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1852200</v>
+      </c>
+      <c r="E10" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>225</v>
+      </c>
+      <c r="F10" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15247310400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>125440</v>
-      </c>
-      <c r="B10">
-        <v>15.049999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>129500</v>
       </c>
       <c r="B11">
         <v>15.049999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D11" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1887871.9999999998</v>
+      </c>
+      <c r="E11" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>226.50249999999997</v>
+      </c>
+      <c r="F11" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15735193600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
+        <v>129500</v>
+      </c>
+      <c r="B12">
+        <v>15.049999999999999</v>
+      </c>
+      <c r="D12" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1948974.9999999998</v>
+      </c>
+      <c r="E12" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>226.50249999999997</v>
+      </c>
+      <c r="F12" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16770250000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>121450</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>15.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="D13" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1833895</v>
+      </c>
+      <c r="E13" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>228.01</v>
+      </c>
+      <c r="F13" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>14750102500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>124250</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>15.35</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="D14" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1907237.5</v>
+      </c>
+      <c r="E14" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>235.6225</v>
+      </c>
+      <c r="F14" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15438062500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>121450</v>
-      </c>
-      <c r="B14">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>119840</v>
       </c>
       <c r="B15">
         <v>15.4</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D15" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1870330</v>
+      </c>
+      <c r="E15" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>237.16000000000003</v>
+      </c>
+      <c r="F15" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>14750102500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
+        <v>119840</v>
+      </c>
+      <c r="B16">
+        <v>15.4</v>
+      </c>
+      <c r="D16" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1845536</v>
+      </c>
+      <c r="E16" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>237.16000000000003</v>
+      </c>
+      <c r="F16" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>14361625600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>124110</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>15.600000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="D17" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1936116.0000000002</v>
+      </c>
+      <c r="E17" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>243.36000000000004</v>
+      </c>
+      <c r="F17" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15403292100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>131040</v>
-      </c>
-      <c r="B17">
-        <v>15.85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>122850</v>
       </c>
       <c r="B18">
         <v>15.85</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D18" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2076984</v>
+      </c>
+      <c r="E18" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>251.2225</v>
+      </c>
+      <c r="F18" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>17171481600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>117180</v>
+        <v>122850</v>
       </c>
       <c r="B19">
         <v>15.85</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D19" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1947172.5</v>
+      </c>
+      <c r="E19" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>251.2225</v>
+      </c>
+      <c r="F19" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15092122500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>128940</v>
+        <v>117180</v>
       </c>
       <c r="B20">
         <v>15.85</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D20" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1857303</v>
+      </c>
+      <c r="E20" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>251.2225</v>
+      </c>
+      <c r="F20" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>13731152400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
+        <v>128940</v>
+      </c>
+      <c r="B21">
+        <v>15.85</v>
+      </c>
+      <c r="D21" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2043699</v>
+      </c>
+      <c r="E21" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>251.2225</v>
+      </c>
+      <c r="F21" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16625523600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>125020</v>
-      </c>
-      <c r="B21">
-        <v>15.95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>123270</v>
       </c>
       <c r="B22">
         <v>15.95</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D22" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1994069</v>
+      </c>
+      <c r="E22" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>254.40249999999997</v>
+      </c>
+      <c r="F22" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15630000400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>120540</v>
+        <v>123270</v>
       </c>
       <c r="B23">
         <v>15.95</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D23" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1966156.5</v>
+      </c>
+      <c r="E23" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>254.40249999999997</v>
+      </c>
+      <c r="F23" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15195492900</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
+        <v>120540</v>
+      </c>
+      <c r="B24">
+        <v>15.95</v>
+      </c>
+      <c r="D24" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1922613</v>
+      </c>
+      <c r="E24" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>254.40249999999997</v>
+      </c>
+      <c r="F24" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>14529891600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>116410</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="D25" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1862560</v>
+      </c>
+      <c r="E25" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>256</v>
+      </c>
+      <c r="F25" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>13551288100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>118090</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>16.05</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="D26" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1895344.5</v>
+      </c>
+      <c r="E26" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>257.60250000000002</v>
+      </c>
+      <c r="F26" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>13945248100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>138180</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>16.200000000000003</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="D27" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2238516.0000000005</v>
+      </c>
+      <c r="E27" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>262.44000000000011</v>
+      </c>
+      <c r="F27" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>19093712400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>127820</v>
-      </c>
-      <c r="B27">
-        <v>16.399999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>125090</v>
       </c>
       <c r="B28">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D28" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2096247.9999999998</v>
+      </c>
+      <c r="E28" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>268.95999999999998</v>
+      </c>
+      <c r="F28" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16337952400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>127470</v>
+        <v>125090</v>
       </c>
       <c r="B29">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D29" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2051475.9999999998</v>
+      </c>
+      <c r="E29" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>268.95999999999998</v>
+      </c>
+      <c r="F29" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15647508100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>141400</v>
+        <v>127470</v>
       </c>
       <c r="B30">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D30" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2090507.9999999998</v>
+      </c>
+      <c r="E30" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>268.95999999999998</v>
+      </c>
+      <c r="F30" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16248600900</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>125580</v>
+        <v>141400</v>
       </c>
       <c r="B31">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D31" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2318960</v>
+      </c>
+      <c r="E31" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>268.95999999999998</v>
+      </c>
+      <c r="F31" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>19993960000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>123830</v>
+        <v>125580</v>
       </c>
       <c r="B32">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D32" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2059511.9999999998</v>
+      </c>
+      <c r="E32" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>268.95999999999998</v>
+      </c>
+      <c r="F32" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15770336400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>135380</v>
+        <v>123830</v>
       </c>
       <c r="B33">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D33" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2030811.9999999998</v>
+      </c>
+      <c r="E33" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>268.95999999999998</v>
+      </c>
+      <c r="F33" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15333868900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
+        <v>135380</v>
+      </c>
+      <c r="B34">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D34" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2220232</v>
+      </c>
+      <c r="E34" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>268.95999999999998</v>
+      </c>
+      <c r="F34" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>18327744400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
         <v>124250</v>
-      </c>
-      <c r="B34">
-        <v>16.45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>129850</v>
       </c>
       <c r="B35">
         <v>16.45</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D35" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2043912.5</v>
+      </c>
+      <c r="E35" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>270.60249999999996</v>
+      </c>
+      <c r="F35" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15438062500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>131600</v>
+        <v>129850</v>
       </c>
       <c r="B36">
         <v>16.45</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D36" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2136032.5</v>
+      </c>
+      <c r="E36" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>270.60249999999996</v>
+      </c>
+      <c r="F36" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16861022500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
+        <v>131600</v>
+      </c>
+      <c r="B37">
+        <v>16.45</v>
+      </c>
+      <c r="D37" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2164820</v>
+      </c>
+      <c r="E37" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>270.60249999999996</v>
+      </c>
+      <c r="F37" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>17318560000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
         <v>129430</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>16.55</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="D38" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2142066.5</v>
+      </c>
+      <c r="E38" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>273.90250000000003</v>
+      </c>
+      <c r="F38" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16752124900</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>126560</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>16.599999999999998</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="D39" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2100895.9999999995</v>
+      </c>
+      <c r="E39" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>275.55999999999995</v>
+      </c>
+      <c r="F39" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16017433600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
         <v>136780</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="D40" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2284226</v>
+      </c>
+      <c r="E40" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>278.89</v>
+      </c>
+      <c r="F40" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>18708768400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>124390</v>
-      </c>
-      <c r="B40">
-        <v>16.850000000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>128170</v>
       </c>
       <c r="B41">
         <v>16.850000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D41" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2095971.5000000002</v>
+      </c>
+      <c r="E41" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>283.92250000000007</v>
+      </c>
+      <c r="F41" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15472872100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>130550</v>
+        <v>128170</v>
       </c>
       <c r="B42">
         <v>16.850000000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D42" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2159664.5</v>
+      </c>
+      <c r="E42" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>283.92250000000007</v>
+      </c>
+      <c r="F42" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16427548900</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
+        <v>130550</v>
+      </c>
+      <c r="B43">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="D43" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2199767.5</v>
+      </c>
+      <c r="E43" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>283.92250000000007</v>
+      </c>
+      <c r="F43" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>17043302500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
         <v>129500</v>
-      </c>
-      <c r="B43">
-        <v>16.899999999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>137620</v>
       </c>
       <c r="B44">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D44" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2188550</v>
+      </c>
+      <c r="E44" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>285.60999999999996</v>
+      </c>
+      <c r="F44" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16770250000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
+        <v>137620</v>
+      </c>
+      <c r="B45">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="D45" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2325778</v>
+      </c>
+      <c r="E45" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>285.60999999999996</v>
+      </c>
+      <c r="F45" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>18939264400</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
         <v>119140</v>
-      </c>
-      <c r="B45">
-        <v>16.95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>139300</v>
       </c>
       <c r="B46">
         <v>16.95</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D46" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2019423</v>
+      </c>
+      <c r="E46" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>287.30249999999995</v>
+      </c>
+      <c r="F46" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>14194339600</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
+        <v>139300</v>
+      </c>
+      <c r="B47">
+        <v>16.95</v>
+      </c>
+      <c r="D47" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2361135</v>
+      </c>
+      <c r="E47" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>287.30249999999995</v>
+      </c>
+      <c r="F47" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>19404490000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
         <v>134750</v>
-      </c>
-      <c r="B47">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>127680</v>
       </c>
       <c r="B48">
         <v>17</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D48" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2290750</v>
+      </c>
+      <c r="E48" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>289</v>
+      </c>
+      <c r="F48" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>18157562500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>136920</v>
+        <v>127680</v>
       </c>
       <c r="B49">
         <v>17</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D49" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2170560</v>
+      </c>
+      <c r="E49" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>289</v>
+      </c>
+      <c r="F49" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16302182400</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
+        <v>136920</v>
+      </c>
+      <c r="B50">
+        <v>17</v>
+      </c>
+      <c r="D50" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2327640</v>
+      </c>
+      <c r="E50" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>289</v>
+      </c>
+      <c r="F50" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>18747086400</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>129990</v>
-      </c>
-      <c r="B50">
-        <v>17.05</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>138530</v>
       </c>
       <c r="B51">
         <v>17.05</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D51" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2216329.5</v>
+      </c>
+      <c r="E51" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>290.70250000000004</v>
+      </c>
+      <c r="F51" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16897400100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>126140</v>
+        <v>138530</v>
       </c>
       <c r="B52">
         <v>17.05</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D52" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2361936.5</v>
+      </c>
+      <c r="E52" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>290.70250000000004</v>
+      </c>
+      <c r="F52" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>19190560900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
+        <v>126140</v>
+      </c>
+      <c r="B53">
+        <v>17.05</v>
+      </c>
+      <c r="D53" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2150687</v>
+      </c>
+      <c r="E53" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>290.70250000000004</v>
+      </c>
+      <c r="F53" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15911299600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
         <v>129850</v>
-      </c>
-      <c r="B53">
-        <v>17.100000000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>133490</v>
       </c>
       <c r="B54">
         <v>17.100000000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D54" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2220435</v>
+      </c>
+      <c r="E54" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>292.41000000000003</v>
+      </c>
+      <c r="F54" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16861022500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>114380</v>
+        <v>133490</v>
       </c>
       <c r="B55">
         <v>17.100000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D55" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2282679</v>
+      </c>
+      <c r="E55" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>292.41000000000003</v>
+      </c>
+      <c r="F55" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>17819580100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
+        <v>114380</v>
+      </c>
+      <c r="B56">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="D56" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>1955898.0000000002</v>
+      </c>
+      <c r="E56" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>292.41000000000003</v>
+      </c>
+      <c r="F56" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>13082784400</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
         <v>131530</v>
       </c>
-      <c r="B56">
+      <c r="B57">
         <v>17.2</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="D57" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2262316</v>
+      </c>
+      <c r="E57" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>295.83999999999997</v>
+      </c>
+      <c r="F57" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>17300140900</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
         <v>132090</v>
-      </c>
-      <c r="B57">
-        <v>17.350000000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>121100</v>
       </c>
       <c r="B58">
         <v>17.350000000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D58" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2291761.5</v>
+      </c>
+      <c r="E58" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>301.02250000000004</v>
+      </c>
+      <c r="F58" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>17447768100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>136710</v>
+        <v>121100</v>
       </c>
       <c r="B59">
         <v>17.350000000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D59" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2101085</v>
+      </c>
+      <c r="E59" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>301.02250000000004</v>
+      </c>
+      <c r="F59" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>14665210000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>124670</v>
+        <v>136710</v>
       </c>
       <c r="B60">
         <v>17.350000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D60" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2371918.5</v>
+      </c>
+      <c r="E60" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>301.02250000000004</v>
+      </c>
+      <c r="F60" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>18689624100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
+        <v>124670</v>
+      </c>
+      <c r="B61">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="D61" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2163024.5</v>
+      </c>
+      <c r="E61" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>301.02250000000004</v>
+      </c>
+      <c r="F61" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15542608900</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
         <v>132370</v>
       </c>
-      <c r="B61">
+      <c r="B62">
         <v>17.399999999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="D62" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2303238</v>
+      </c>
+      <c r="E62" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>302.75999999999993</v>
+      </c>
+      <c r="F62" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>17521816900</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
         <v>137480</v>
-      </c>
-      <c r="B62">
-        <v>17.450000000000003</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>126560</v>
       </c>
       <c r="B63">
         <v>17.450000000000003</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D63" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2399026.0000000005</v>
+      </c>
+      <c r="E63" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>304.50250000000011</v>
+      </c>
+      <c r="F63" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>18900750400</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
+        <v>126560</v>
+      </c>
+      <c r="B64">
+        <v>17.450000000000003</v>
+      </c>
+      <c r="D64" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2208472.0000000005</v>
+      </c>
+      <c r="E64" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>304.50250000000011</v>
+      </c>
+      <c r="F64" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16017433600</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
         <v>132510</v>
       </c>
-      <c r="B64">
+      <c r="B65">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65">
+      <c r="D65" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2318925</v>
+      </c>
+      <c r="E65" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>306.25</v>
+      </c>
+      <c r="F65" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>17558900100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
         <v>142870</v>
-      </c>
-      <c r="B65">
-        <v>17.549999999999997</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <v>132510</v>
       </c>
       <c r="B66">
         <v>17.549999999999997</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D66" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2507368.4999999995</v>
+      </c>
+      <c r="E66" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>308.00249999999988</v>
+      </c>
+      <c r="F66" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>20411836900</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
+        <v>132510</v>
+      </c>
+      <c r="B67">
+        <v>17.549999999999997</v>
+      </c>
+      <c r="D67" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2325550.4999999995</v>
+      </c>
+      <c r="E67" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>308.00249999999988</v>
+      </c>
+      <c r="F67" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>17558900100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68">
         <v>128240</v>
-      </c>
-      <c r="B67">
-        <v>17.600000000000001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>129500</v>
       </c>
       <c r="B68">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D68" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2257024</v>
+      </c>
+      <c r="E68" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>309.76000000000005</v>
+      </c>
+      <c r="F68" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16445497600</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
+        <v>129500</v>
+      </c>
+      <c r="B69">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D69" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2279200</v>
+      </c>
+      <c r="E69" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>309.76000000000005</v>
+      </c>
+      <c r="F69" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16770250000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70">
         <v>135380</v>
       </c>
-      <c r="B69">
+      <c r="B70">
         <v>17.7</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70">
+      <c r="D70" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2396226</v>
+      </c>
+      <c r="E70" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>313.28999999999996</v>
+      </c>
+      <c r="F70" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>18327744400</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71">
         <v>130270</v>
-      </c>
-      <c r="B70">
-        <v>17.899999999999999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <v>135170</v>
       </c>
       <c r="B71">
         <v>17.899999999999999</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D71" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2331833</v>
+      </c>
+      <c r="E71" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>320.40999999999997</v>
+      </c>
+      <c r="F71" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>16970272900</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
+        <v>135170</v>
+      </c>
+      <c r="B72">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D72" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2419543</v>
+      </c>
+      <c r="E72" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>320.40999999999997</v>
+      </c>
+      <c r="F72" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>18270928900</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73">
         <v>135310</v>
-      </c>
-      <c r="B72">
-        <v>17.95</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>124460</v>
       </c>
       <c r="B73">
         <v>17.95</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D73" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2428814.5</v>
+      </c>
+      <c r="E73" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>322.20249999999999</v>
+      </c>
+      <c r="F73" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>18308796100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
+        <v>124460</v>
+      </c>
+      <c r="B74">
+        <v>17.95</v>
+      </c>
+      <c r="D74" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2234057</v>
+      </c>
+      <c r="E74" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>322.20249999999999</v>
+      </c>
+      <c r="F74" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>15490291600</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75">
         <v>138250</v>
-      </c>
-      <c r="B74">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <v>135380</v>
       </c>
       <c r="B75">
         <v>18</v>
       </c>
+      <c r="D75" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2488500</v>
+      </c>
+      <c r="E75" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>324</v>
+      </c>
+      <c r="F75" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>19113062500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>135380</v>
+      </c>
+      <c r="B76">
+        <v>18</v>
+      </c>
+      <c r="D76" s="7">
+        <f>Table1[[#This Row],[Salary]]*Table1[[#This Row],[Years Employed]]</f>
+        <v>2436840</v>
+      </c>
+      <c r="E76" s="7">
+        <f>Table1[[#This Row],[Years Employed]]^2</f>
+        <v>324</v>
+      </c>
+      <c r="F76" s="7">
+        <f>Table1[[#This Row],[Salary]]^2</f>
+        <v>18327744400</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="7">
+        <f t="shared" ref="A77:B77" si="0">SUM(A3:A76)</f>
+        <v>9475340</v>
+      </c>
+      <c r="B77" s="7">
+        <f t="shared" si="0"/>
+        <v>1213.9500000000003</v>
+      </c>
+      <c r="C77" t="s">
+        <v>35</v>
+      </c>
+      <c r="D77" s="8">
+        <f>SUM(D3:D76)</f>
+        <v>155796182.5</v>
+      </c>
+      <c r="E77" s="8">
+        <f t="shared" ref="E77:F77" si="1">SUM(E3:E76)</f>
+        <v>20028.917499999996</v>
+      </c>
+      <c r="F77" s="8">
+        <f t="shared" si="1"/>
+        <v>1216649694400</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
sync for ep 3
</commit_message>
<xml_diff>
--- a/notebooks/SOSNEP03LR.xlsx
+++ b/notebooks/SOSNEP03LR.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwoody\repos\dataexposed\notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\dataexposed\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9B0066-743E-4FD6-82B3-DE06EBA9FF19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37B9CA1-CF63-466E-B89F-E2E2AFF1206B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" tabRatio="255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="255" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="3" r:id="rId1"/>
     <sheet name="DataTable" sheetId="2" r:id="rId2"/>
-    <sheet name="Salries" sheetId="1" r:id="rId3"/>
+    <sheet name="Salaries" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">DataTable!$A$1:$B$75</definedName>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Salary</t>
   </si>
@@ -169,7 +169,10 @@
     <t>Step 3: Build the Formula y=a+bx:</t>
   </si>
   <si>
-    <t>y=3.63E-10*1.46E-11*x</t>
+    <t>y=77024+3110x</t>
+  </si>
+  <si>
+    <t>Slope</t>
   </si>
 </sst>
 </file>
@@ -2666,35 +2669,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E3CB93-47D2-4365-A164-607BEBECA4E7}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>0.57085779654949864</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>0.32587862388134881</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2718,7 +2721,7 @@
         <v>0.31638395661207203</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2726,7 +2729,7 @@
         <v>5608.1827582952183</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2734,12 +2737,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>13</v>
@@ -2757,7 +2760,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2777,7 +2780,7 @@
         <v>1.3393657026533788E-7</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2793,7 +2796,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -2807,8 +2810,8 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>18</v>
@@ -2835,7 +2838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -2864,7 +2867,7 @@
         <v>91536.175445194982</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>12</v>
       </c>
@@ -2893,13 +2896,13 @@
         <v>4524.6816432578671</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
@@ -2910,7 +2913,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -2921,7 +2924,7 @@
         <v>1371.8820962593309</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -2932,7 +2935,7 @@
         <v>7754.3072626506328</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -2943,7 +2946,7 @@
         <v>-871.44107343631913</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>4</v>
       </c>
@@ -2954,7 +2957,7 @@
         <v>-1830.5278246754315</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>5</v>
       </c>
@@ -2965,7 +2968,7 @@
         <v>-4790.8271591102093</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>6</v>
       </c>
@@ -2976,7 +2979,7 @@
         <v>270.08608965066378</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>7</v>
       </c>
@@ -2987,7 +2990,7 @@
         <v>270.08608965066378</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>8</v>
       </c>
@@ -2998,7 +3001,7 @@
         <v>2061.2986728463293</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>9</v>
       </c>
@@ -3009,7 +3012,7 @@
         <v>6121.2986728463293</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>10</v>
       </c>
@@ -3020,7 +3023,7 @@
         <v>-2097.4887439580198</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>11</v>
       </c>
@@ -3031,7 +3034,7 @@
         <v>-141.42582797975047</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>12</v>
       </c>
@@ -3042,7 +3045,7 @@
         <v>-3110.2132447840995</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>13</v>
       </c>
@@ -3053,7 +3056,7 @@
         <v>-4720.2132447840995</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>14</v>
       </c>
@@ -3064,7 +3067,7 @@
         <v>-1125.3629120014957</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>15</v>
       </c>
@@ -3075,7 +3078,7 @@
         <v>4960.7000039767736</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>16</v>
       </c>
@@ -3086,7 +3089,7 @@
         <v>-3229.2999960232264</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>17</v>
       </c>
@@ -3097,7 +3100,7 @@
         <v>-8899.2999960232264</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>18</v>
       </c>
@@ -3108,7 +3111,7 @@
         <v>2860.7000039767736</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>19</v>
       </c>
@@ -3119,7 +3122,7 @@
         <v>-1396.87482963191</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>20</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>-3146.87482963191</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>21</v>
       </c>
@@ -3141,7 +3144,7 @@
         <v>-5876.87482963191</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>22</v>
       </c>
@@ -3152,7 +3155,7 @@
         <v>-10175.662246436259</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>23</v>
       </c>
@@ -3163,7 +3166,7 @@
         <v>-8664.4496632406081</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>24</v>
       </c>
@@ -3174,7 +3177,7 @@
         <v>10919.188086346345</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>25</v>
       </c>
@@ -3185,7 +3188,7 @@
         <v>-115.96158087103686</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>26</v>
       </c>
@@ -3196,7 +3199,7 @@
         <v>-2845.9615808710369</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>27</v>
       </c>
@@ -3207,7 +3210,7 @@
         <v>-465.96158087103686</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>28</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>13464.038419128963</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>29</v>
       </c>
@@ -3229,7 +3232,7 @@
         <v>-2355.9615808710369</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>30</v>
       </c>
@@ -3240,7 +3243,7 @@
         <v>-4105.9615808710369</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>31</v>
       </c>
@@ -3251,7 +3254,7 @@
         <v>7444.0384191289631</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>32</v>
       </c>
@@ -3262,7 +3265,7 @@
         <v>-3854.7489976753859</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>33</v>
       </c>
@@ -3273,7 +3276,7 @@
         <v>1745.2510023246141</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>34</v>
       </c>
@@ -3284,7 +3287,7 @@
         <v>3495.2510023246141</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>35</v>
       </c>
@@ -3295,7 +3298,7 @@
         <v>987.67616871591599</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>36</v>
       </c>
@@ -3306,7 +3309,7 @@
         <v>-2051.1112480884185</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>37</v>
       </c>
@@ -3317,7 +3320,7 @@
         <v>7831.3139183028834</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>38</v>
       </c>
@@ -3328,7 +3331,7 @@
         <v>-5065.0483321101638</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>39</v>
       </c>
@@ -3339,7 +3342,7 @@
         <v>-1285.0483321101638</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>40</v>
       </c>
@@ -3350,7 +3353,7 @@
         <v>1094.9516678898362</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>41</v>
       </c>
@@ -3361,7 +3364,7 @@
         <v>-123.83574891451281</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>42</v>
       </c>
@@ -3372,7 +3375,7 @@
         <v>7996.1642510854872</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43</v>
       </c>
@@ -3383,7 +3386,7 @@
         <v>-10652.623165718862</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44</v>
       </c>
@@ -3394,7 +3397,7 @@
         <v>9507.3768342811381</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45</v>
       </c>
@@ -3405,7 +3408,7 @@
         <v>4788.5894174767891</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>46</v>
       </c>
@@ -3416,7 +3419,7 @@
         <v>-2281.4105825232109</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>47</v>
       </c>
@@ -3427,7 +3430,7 @@
         <v>6958.5894174767891</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>48</v>
       </c>
@@ -3438,7 +3441,7 @@
         <v>-140.19799932755996</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>49</v>
       </c>
@@ -3449,7 +3452,7 @@
         <v>8399.80200067244</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>50</v>
       </c>
@@ -3460,7 +3463,7 @@
         <v>-3990.19799932756</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>51</v>
       </c>
@@ -3471,7 +3474,7 @@
         <v>-448.98541613190901</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>52</v>
       </c>
@@ -3482,7 +3485,7 @@
         <v>3191.014583868091</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>53</v>
       </c>
@@ -3493,7 +3496,7 @@
         <v>-15918.985416131909</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>54</v>
       </c>
@@ -3504,7 +3507,7 @@
         <v>893.43975025940745</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>55</v>
       </c>
@@ -3515,7 +3518,7 @@
         <v>947.07749984634575</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>56</v>
       </c>
@@ -3526,7 +3529,7 @@
         <v>-10042.922500153654</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>57</v>
       </c>
@@ -3537,7 +3540,7 @@
         <v>5567.0774998463457</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>58</v>
       </c>
@@ -3548,7 +3551,7 @@
         <v>-6472.9225001536543</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>59</v>
       </c>
@@ -3559,7 +3562,7 @@
         <v>1058.2900830420258</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>60</v>
       </c>
@@ -3570,7 +3573,7 @@
         <v>5999.5026662376476</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>61</v>
       </c>
@@ -3581,7 +3584,7 @@
         <v>-4920.4973337623524</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>62</v>
       </c>
@@ -3592,7 +3595,7 @@
         <v>860.7152494333277</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>63</v>
       </c>
@@ -3603,7 +3606,7 @@
         <v>11051.927832629008</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>64</v>
       </c>
@@ -3614,7 +3617,7 @@
         <v>691.92783262900775</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>65</v>
       </c>
@@ -3625,7 +3628,7 @@
         <v>-3746.8595841753704</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>66</v>
       </c>
@@ -3636,7 +3639,7 @@
         <v>-2486.8595841753704</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>67</v>
       </c>
@@ -3647,7 +3650,7 @@
         <v>3055.5655822159315</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>68</v>
       </c>
@@ -3658,7 +3661,7 @@
         <v>-2729.5840850014356</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>69</v>
       </c>
@@ -3669,7 +3672,7 @@
         <v>2170.4159149985644</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>70</v>
       </c>
@@ -3680,7 +3683,7 @@
         <v>2141.6284981942154</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>71</v>
       </c>
@@ -3691,7 +3694,7 @@
         <v>-8708.3715018057846</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>72</v>
       </c>
@@ -3702,7 +3705,7 @@
         <v>4912.8410813898663</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>73</v>
       </c>
@@ -3727,13 +3730,13 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3741,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>119980</v>
       </c>
@@ -3749,7 +3752,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>116480</v>
       </c>
@@ -3757,7 +3760,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>123200</v>
       </c>
@@ -3765,7 +3768,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>117950</v>
       </c>
@@ -3773,7 +3776,7 @@
         <v>13.700000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>118510</v>
       </c>
@@ -3781,7 +3784,7 @@
         <v>14.15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>116900</v>
       </c>
@@ -3789,7 +3792,7 @@
         <v>14.55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>123480</v>
       </c>
@@ -3797,7 +3800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>123480</v>
       </c>
@@ -3805,7 +3808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>125440</v>
       </c>
@@ -3813,7 +3816,7 @@
         <v>15.049999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>129500</v>
       </c>
@@ -3821,7 +3824,7 @@
         <v>15.049999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>121450</v>
       </c>
@@ -3829,7 +3832,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>124250</v>
       </c>
@@ -3837,7 +3840,7 @@
         <v>15.35</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>121450</v>
       </c>
@@ -3845,7 +3848,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>119840</v>
       </c>
@@ -3853,7 +3856,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>124110</v>
       </c>
@@ -3861,7 +3864,7 @@
         <v>15.600000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>131040</v>
       </c>
@@ -3869,7 +3872,7 @@
         <v>15.85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>122850</v>
       </c>
@@ -3877,7 +3880,7 @@
         <v>15.85</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>117180</v>
       </c>
@@ -3885,7 +3888,7 @@
         <v>15.85</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>128940</v>
       </c>
@@ -3893,7 +3896,7 @@
         <v>15.85</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>125020</v>
       </c>
@@ -3901,7 +3904,7 @@
         <v>15.95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>123270</v>
       </c>
@@ -3909,7 +3912,7 @@
         <v>15.95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>120540</v>
       </c>
@@ -3917,7 +3920,7 @@
         <v>15.95</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>116410</v>
       </c>
@@ -3925,7 +3928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>118090</v>
       </c>
@@ -3933,7 +3936,7 @@
         <v>16.05</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>138180</v>
       </c>
@@ -3941,7 +3944,7 @@
         <v>16.200000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>127820</v>
       </c>
@@ -3949,7 +3952,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>125090</v>
       </c>
@@ -3957,7 +3960,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>127470</v>
       </c>
@@ -3965,7 +3968,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>141400</v>
       </c>
@@ -3973,7 +3976,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>125580</v>
       </c>
@@ -3981,7 +3984,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>123830</v>
       </c>
@@ -3989,7 +3992,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>135380</v>
       </c>
@@ -3997,7 +4000,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>124250</v>
       </c>
@@ -4005,7 +4008,7 @@
         <v>16.45</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>129850</v>
       </c>
@@ -4013,7 +4016,7 @@
         <v>16.45</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>131600</v>
       </c>
@@ -4021,7 +4024,7 @@
         <v>16.45</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>129430</v>
       </c>
@@ -4029,7 +4032,7 @@
         <v>16.55</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>126560</v>
       </c>
@@ -4037,7 +4040,7 @@
         <v>16.599999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>136780</v>
       </c>
@@ -4045,7 +4048,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>124390</v>
       </c>
@@ -4053,7 +4056,7 @@
         <v>16.850000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>128170</v>
       </c>
@@ -4061,7 +4064,7 @@
         <v>16.850000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>130550</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>16.850000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>129500</v>
       </c>
@@ -4077,7 +4080,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>137620</v>
       </c>
@@ -4085,7 +4088,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>119140</v>
       </c>
@@ -4093,7 +4096,7 @@
         <v>16.95</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>139300</v>
       </c>
@@ -4101,7 +4104,7 @@
         <v>16.95</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>134750</v>
       </c>
@@ -4109,7 +4112,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>127680</v>
       </c>
@@ -4117,7 +4120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>136920</v>
       </c>
@@ -4125,7 +4128,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>129990</v>
       </c>
@@ -4133,7 +4136,7 @@
         <v>17.05</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>138530</v>
       </c>
@@ -4141,7 +4144,7 @@
         <v>17.05</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>126140</v>
       </c>
@@ -4149,7 +4152,7 @@
         <v>17.05</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>129850</v>
       </c>
@@ -4157,7 +4160,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>133490</v>
       </c>
@@ -4165,7 +4168,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>114380</v>
       </c>
@@ -4173,7 +4176,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>131530</v>
       </c>
@@ -4181,7 +4184,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>132090</v>
       </c>
@@ -4189,7 +4192,7 @@
         <v>17.350000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>121100</v>
       </c>
@@ -4197,7 +4200,7 @@
         <v>17.350000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>136710</v>
       </c>
@@ -4205,7 +4208,7 @@
         <v>17.350000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>124670</v>
       </c>
@@ -4213,7 +4216,7 @@
         <v>17.350000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>132370</v>
       </c>
@@ -4221,7 +4224,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>137480</v>
       </c>
@@ -4229,7 +4232,7 @@
         <v>17.450000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>126560</v>
       </c>
@@ -4237,7 +4240,7 @@
         <v>17.450000000000003</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>132510</v>
       </c>
@@ -4245,7 +4248,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>142870</v>
       </c>
@@ -4253,7 +4256,7 @@
         <v>17.549999999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>132510</v>
       </c>
@@ -4261,7 +4264,7 @@
         <v>17.549999999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>128240</v>
       </c>
@@ -4269,7 +4272,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>129500</v>
       </c>
@@ -4277,7 +4280,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>135380</v>
       </c>
@@ -4285,7 +4288,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>130270</v>
       </c>
@@ -4293,7 +4296,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>135170</v>
       </c>
@@ -4301,7 +4304,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>135310</v>
       </c>
@@ -4309,7 +4312,7 @@
         <v>17.95</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>124460</v>
       </c>
@@ -4317,7 +4320,7 @@
         <v>17.95</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>138250</v>
       </c>
@@ -4325,7 +4328,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>135380</v>
       </c>
@@ -4345,24 +4348,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.88671875" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>37</v>
       </c>
@@ -4380,11 +4383,14 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
       <c r="P1" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4413,10 +4419,10 @@
       </c>
       <c r="N2" s="9">
         <f>L2/L3</f>
-        <v>3.63011599035688E-10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+        <v>77023.611242611383</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>119980</v>
       </c>
@@ -4440,15 +4446,19 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9">
-        <f>(COUNT(Table1[Salary])*(D77^2))-((Table1[[#Totals],[Years Employed]]^2))</f>
-        <v>1.7961613356349509E+18</v>
+        <f>(COUNT(Table1[Salary])*(E77))-((Table1[[#Totals],[Years Employed]]^2))</f>
+        <v>8465.2924999990501</v>
       </c>
       <c r="M3" s="9"/>
+      <c r="N3">
+        <f>INTERCEPT(Table1[Salary],Table1[Years Employed])</f>
+        <v>77023.611242612154</v>
+      </c>
       <c r="P3" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>116480</v>
       </c>
@@ -4473,8 +4483,11 @@
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
-    </row>
-    <row r="5" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="N4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>123200</v>
       </c>
@@ -4506,10 +4519,10 @@
       </c>
       <c r="N5" s="9">
         <f>L5/L6</f>
-        <v>1.4658211084746934E-11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>3110.1715622940433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>117950</v>
       </c>
@@ -4533,12 +4546,16 @@
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9">
-        <f>(COUNT(Table1[Salary])*(D77^2))-(Table1[[#Totals],[Years Employed]]^2)</f>
-        <v>1.7961613356349509E+18</v>
+        <f>(COUNT(Table1[Salary])*(E77))-(Table1[[#Totals],[Years Employed]]^2)</f>
+        <v>8465.2924999990501</v>
       </c>
       <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <f>SLOPE(Table1[Salary],Table1[Years Employed])</f>
+        <v>3110.1715622939155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>118510</v>
       </c>
@@ -4564,7 +4581,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>116900</v>
       </c>
@@ -4584,7 +4601,7 @@
         <v>13665610000</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>123480</v>
       </c>
@@ -4604,7 +4621,7 @@
         <v>15247310400</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>123480</v>
       </c>
@@ -4624,7 +4641,7 @@
         <v>15247310400</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>125440</v>
       </c>
@@ -4644,7 +4661,7 @@
         <v>15735193600</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>129500</v>
       </c>
@@ -4664,7 +4681,7 @@
         <v>16770250000</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>121450</v>
       </c>
@@ -4684,7 +4701,7 @@
         <v>14750102500</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>124250</v>
       </c>
@@ -4704,7 +4721,7 @@
         <v>15438062500</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>121450</v>
       </c>
@@ -4724,7 +4741,7 @@
         <v>14750102500</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>119840</v>
       </c>
@@ -4744,7 +4761,7 @@
         <v>14361625600</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>124110</v>
       </c>
@@ -4764,7 +4781,7 @@
         <v>15403292100</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>131040</v>
       </c>
@@ -4784,7 +4801,7 @@
         <v>17171481600</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>122850</v>
       </c>
@@ -4804,7 +4821,7 @@
         <v>15092122500</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>117180</v>
       </c>
@@ -4824,7 +4841,7 @@
         <v>13731152400</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>128940</v>
       </c>
@@ -4844,7 +4861,7 @@
         <v>16625523600</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>125020</v>
       </c>
@@ -4864,7 +4881,7 @@
         <v>15630000400</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>123270</v>
       </c>
@@ -4884,7 +4901,7 @@
         <v>15195492900</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>120540</v>
       </c>
@@ -4904,7 +4921,7 @@
         <v>14529891600</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>116410</v>
       </c>
@@ -4924,7 +4941,7 @@
         <v>13551288100</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>118090</v>
       </c>
@@ -4944,7 +4961,7 @@
         <v>13945248100</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>138180</v>
       </c>
@@ -4964,7 +4981,7 @@
         <v>19093712400</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>127820</v>
       </c>
@@ -4984,7 +5001,7 @@
         <v>16337952400</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>125090</v>
       </c>
@@ -5004,7 +5021,7 @@
         <v>15647508100</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>127470</v>
       </c>
@@ -5024,7 +5041,7 @@
         <v>16248600900</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>141400</v>
       </c>
@@ -5044,7 +5061,7 @@
         <v>19993960000</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>125580</v>
       </c>
@@ -5064,7 +5081,7 @@
         <v>15770336400</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>123830</v>
       </c>
@@ -5084,7 +5101,7 @@
         <v>15333868900</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>135380</v>
       </c>
@@ -5104,7 +5121,7 @@
         <v>18327744400</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>124250</v>
       </c>
@@ -5124,7 +5141,7 @@
         <v>15438062500</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>129850</v>
       </c>
@@ -5144,7 +5161,7 @@
         <v>16861022500</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>131600</v>
       </c>
@@ -5164,7 +5181,7 @@
         <v>17318560000</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>129430</v>
       </c>
@@ -5184,7 +5201,7 @@
         <v>16752124900</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>126560</v>
       </c>
@@ -5204,7 +5221,7 @@
         <v>16017433600</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>136780</v>
       </c>
@@ -5224,7 +5241,7 @@
         <v>18708768400</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>124390</v>
       </c>
@@ -5244,7 +5261,7 @@
         <v>15472872100</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>128170</v>
       </c>
@@ -5264,7 +5281,7 @@
         <v>16427548900</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>130550</v>
       </c>
@@ -5284,7 +5301,7 @@
         <v>17043302500</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>129500</v>
       </c>
@@ -5304,7 +5321,7 @@
         <v>16770250000</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>137620</v>
       </c>
@@ -5324,7 +5341,7 @@
         <v>18939264400</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>119140</v>
       </c>
@@ -5344,7 +5361,7 @@
         <v>14194339600</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>139300</v>
       </c>
@@ -5364,7 +5381,7 @@
         <v>19404490000</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>134750</v>
       </c>
@@ -5384,7 +5401,7 @@
         <v>18157562500</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>127680</v>
       </c>
@@ -5404,7 +5421,7 @@
         <v>16302182400</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>136920</v>
       </c>
@@ -5424,7 +5441,7 @@
         <v>18747086400</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>129990</v>
       </c>
@@ -5444,7 +5461,7 @@
         <v>16897400100</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>138530</v>
       </c>
@@ -5464,7 +5481,7 @@
         <v>19190560900</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>126140</v>
       </c>
@@ -5484,7 +5501,7 @@
         <v>15911299600</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>129850</v>
       </c>
@@ -5504,7 +5521,7 @@
         <v>16861022500</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>133490</v>
       </c>
@@ -5524,7 +5541,7 @@
         <v>17819580100</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>114380</v>
       </c>
@@ -5544,7 +5561,7 @@
         <v>13082784400</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>131530</v>
       </c>
@@ -5564,7 +5581,7 @@
         <v>17300140900</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>132090</v>
       </c>
@@ -5584,7 +5601,7 @@
         <v>17447768100</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>121100</v>
       </c>
@@ -5604,7 +5621,7 @@
         <v>14665210000</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>136710</v>
       </c>
@@ -5624,7 +5641,7 @@
         <v>18689624100</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>124670</v>
       </c>
@@ -5644,7 +5661,7 @@
         <v>15542608900</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>132370</v>
       </c>
@@ -5664,7 +5681,7 @@
         <v>17521816900</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>137480</v>
       </c>
@@ -5684,7 +5701,7 @@
         <v>18900750400</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>126560</v>
       </c>
@@ -5704,7 +5721,7 @@
         <v>16017433600</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>132510</v>
       </c>
@@ -5724,7 +5741,7 @@
         <v>17558900100</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>142870</v>
       </c>
@@ -5744,7 +5761,7 @@
         <v>20411836900</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>132510</v>
       </c>
@@ -5764,7 +5781,7 @@
         <v>17558900100</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>128240</v>
       </c>
@@ -5784,7 +5801,7 @@
         <v>16445497600</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>129500</v>
       </c>
@@ -5804,7 +5821,7 @@
         <v>16770250000</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>135380</v>
       </c>
@@ -5824,7 +5841,7 @@
         <v>18327744400</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>130270</v>
       </c>
@@ -5844,7 +5861,7 @@
         <v>16970272900</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>135170</v>
       </c>
@@ -5864,7 +5881,7 @@
         <v>18270928900</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>135310</v>
       </c>
@@ -5884,7 +5901,7 @@
         <v>18308796100</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>124460</v>
       </c>
@@ -5904,7 +5921,7 @@
         <v>15490291600</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>138250</v>
       </c>
@@ -5924,7 +5941,7 @@
         <v>19113062500</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>135380</v>
       </c>
@@ -5944,7 +5961,7 @@
         <v>18327744400</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <f t="shared" ref="A77:B77" si="0">SUM(A3:A76)</f>
         <v>9475340</v>

</xml_diff>